<commit_message>
Trash and Table Fix
</commit_message>
<xml_diff>
--- a/public/excel_files/masterlist-2014-09-29.xlsx
+++ b/public/excel_files/masterlist-2014-09-29.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="31">
   <si>
     <t>Payroll Period</t>
   </si>
@@ -105,12 +105,6 @@
   </si>
   <si>
     <t>13,500.00</t>
-  </si>
-  <si>
-    <t>2,052.00</t>
-  </si>
-  <si>
-    <t>3,181.59</t>
   </si>
   <si>
     <t>Jen Dee  Dela Cruz</t>
@@ -621,19 +615,19 @@
         <v>50</v>
       </c>
       <c r="M5">
-        <v>5769.23076923077</v>
-      </c>
-      <c r="N5" t="s">
-        <v>30</v>
+        <v>11538.46153846154</v>
+      </c>
+      <c r="N5">
+        <v>0</v>
       </c>
       <c r="O5">
-        <v>72</v>
+        <v>0</v>
       </c>
       <c r="P5" t="s">
         <v>28</v>
       </c>
-      <c r="Q5" t="s">
-        <v>31</v>
+      <c r="Q5">
+        <v>465.67</v>
       </c>
     </row>
     <row r="6" spans="1:17">
@@ -644,7 +638,7 @@
         <v>6</v>
       </c>
       <c r="C6" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D6">
         <v>24</v>
@@ -674,7 +668,7 @@
         <v>50</v>
       </c>
       <c r="M6">
-        <v>12692.30769230769</v>
+        <v>11538.46153846154</v>
       </c>
       <c r="N6">
         <v>0</v>
@@ -686,7 +680,7 @@
         <v>0</v>
       </c>
       <c r="Q6">
-        <v>-532.96</v>
+        <v>620.89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>